<commit_message>
Cambio de árbol a markmap
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2a9e946ecd1f9e6/DNP - Guía de buenas practicas Genero - IA/Seguimiento técnico -contrato 1104-2024 DNP/Entregables/Entregable 3/Catalogo de herramientas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFBFDB5B-C258-4359-9D42-4241170BE225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{162360D0-3BFD-4227-92E7-425547173B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13613,8 +13613,8 @@
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="E31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+      <pane ySplit="1" topLeftCell="D29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -14558,7 +14558,7 @@
         <v>144</v>
       </c>
       <c r="I32" s="103" t="s">
-        <v>955</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="43.5">
@@ -14587,7 +14587,7 @@
         <v>144</v>
       </c>
       <c r="I33" s="103" t="s">
-        <v>955</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="45.75">

</xml_diff>